<commit_message>
Updated expense report with latest Amazon order and revised HobbyKing order with refunded motors
</commit_message>
<xml_diff>
--- a/Ordered Parts/Expense Report.xlsx
+++ b/Ordered Parts/Expense Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t>Description</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Arrow Order 4.pdf</t>
   </si>
   <si>
-    <t>Hobby King Order 4.pdf</t>
-  </si>
-  <si>
     <t>Total Expenses</t>
   </si>
   <si>
@@ -243,13 +240,31 @@
     <t>Amazon Order 8.pdf</t>
   </si>
   <si>
-    <t>Amazon Order 9.pdf</t>
-  </si>
-  <si>
     <t>Mounting screws, nuts, and standoffs, AC/DC Power Adapter, Programming Cable, and Ball Bearings</t>
   </si>
   <si>
     <t>*Not sure whether to expense this order</t>
+  </si>
+  <si>
+    <t>Hobby King Order 4.pdf**</t>
+  </si>
+  <si>
+    <t>Amazon Order 10</t>
+  </si>
+  <si>
+    <t>Amazon Order 10.pdf</t>
+  </si>
+  <si>
+    <t>Female PCB Headers, 2mm Bullet Plugs, M3 screws</t>
+  </si>
+  <si>
+    <t>Amazon Order 9.pdf***</t>
+  </si>
+  <si>
+    <t>***Refunded $8.18 for an incorrect shipment</t>
+  </si>
+  <si>
+    <t>**Refunded $23.58 after 2 motors were out of stock</t>
   </si>
 </sst>
 </file>
@@ -596,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1003,13 +1018,14 @@
         <v>63</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E20" s="6">
-        <v>2139.12</v>
+        <f>2139.12-23.58</f>
+        <v>2115.54</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1023,18 +1039,18 @@
         <v>63</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" s="6">
         <v>387.12</v>
       </c>
       <c r="F21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="5">
         <v>43150</v>
@@ -1043,13 +1059,14 @@
         <v>63</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E22" s="6">
-        <v>1537.58</v>
+        <f>1537.58-8.18</f>
+        <v>1529.3999999999999</v>
       </c>
       <c r="F22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1073,17 +1090,45 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D24" s="1" t="s">
-        <v>69</v>
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="5">
+        <v>43153</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="E24" s="6">
-        <f>SUM(E2:E23)</f>
-        <v>5206.1699999999992</v>
+        <v>101.29</v>
+      </c>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="6">
+        <f>SUM(E2:E24)</f>
+        <v>5275.6999999999989</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>76</v>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1107,11 +1152,12 @@
     <hyperlink ref="D17" r:id="rId17" xr:uid="{70D213E5-2585-44D5-92CC-E6C60541605E}"/>
     <hyperlink ref="D23" r:id="rId18" xr:uid="{66E46976-B18D-456B-A336-0B5FE78797A2}"/>
     <hyperlink ref="D19" r:id="rId19" xr:uid="{0A5E70A2-D3DA-4F6F-8971-50C839EF0023}"/>
-    <hyperlink ref="D20" r:id="rId20" xr:uid="{83BDE046-A90B-406F-82B1-D772911E27C4}"/>
+    <hyperlink ref="D20" r:id="rId20" display="Hobby King Order 4.pdf" xr:uid="{83BDE046-A90B-406F-82B1-D772911E27C4}"/>
     <hyperlink ref="D21" r:id="rId21" xr:uid="{B3A30BFC-C2B1-4D29-98C5-8BFED13079CB}"/>
-    <hyperlink ref="D22" r:id="rId22" xr:uid="{AABADA5C-D5EF-4946-BC2E-666040306F4F}"/>
+    <hyperlink ref="D22" r:id="rId22" display="Amazon Order 9.pdf" xr:uid="{AABADA5C-D5EF-4946-BC2E-666040306F4F}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{A711B88F-8C4F-431B-94A6-4849A4C6E732}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added invoice from latest Arrow order to expense report
</commit_message>
<xml_diff>
--- a/Ordered Parts/Expense Report.xlsx
+++ b/Ordered Parts/Expense Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="91">
   <si>
     <t>Description</t>
   </si>
@@ -283,6 +283,15 @@
   </si>
   <si>
     <t>JLCPCB Order.pdf</t>
+  </si>
+  <si>
+    <t>Arrow Order 5.pdf</t>
+  </si>
+  <si>
+    <t>PCB Manufacturing</t>
+  </si>
+  <si>
+    <t>Longer Programming Cables</t>
   </si>
 </sst>
 </file>
@@ -632,7 +641,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,7 +1146,9 @@
       <c r="C25" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="E25" s="6">
         <v>58.73</v>
       </c>
@@ -1161,6 +1172,9 @@
       <c r="E26" s="6">
         <v>209.04</v>
       </c>
+      <c r="F26" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1177,6 +1191,9 @@
       </c>
       <c r="E27" s="6">
         <v>58.07</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1228,8 +1245,9 @@
     <hyperlink ref="D24" r:id="rId23" xr:uid="{A711B88F-8C4F-431B-94A6-4849A4C6E732}"/>
     <hyperlink ref="D26" r:id="rId24" xr:uid="{078ADCB4-68C8-47D6-921B-BFCF3D41E25D}"/>
     <hyperlink ref="D27" r:id="rId25" xr:uid="{D0FFA605-99F2-48D2-A9AC-D83405F41AFA}"/>
+    <hyperlink ref="D25" r:id="rId26" xr:uid="{0958646A-9138-4386-A3D4-B440EC4F598E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId26"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added most recent Amazon order invoice to expense report
</commit_message>
<xml_diff>
--- a/Ordered Parts/Expense Report.xlsx
+++ b/Ordered Parts/Expense Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
   <si>
     <t>Description</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t>Longer Programming Cables</t>
+  </si>
+  <si>
+    <t>Amazon Order 12</t>
+  </si>
+  <si>
+    <t>Amazon Order 12.pdf</t>
+  </si>
+  <si>
+    <t>12V Power Adapters</t>
   </si>
 </sst>
 </file>
@@ -638,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,24 +1206,44 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D28" s="1" t="s">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="5">
+        <v>43158</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="6">
+        <v>27.97</v>
+      </c>
+      <c r="F28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="6">
-        <f>SUM(E2:E27)</f>
-        <v>5275.5399999999981</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
+      <c r="E29" s="6">
+        <f>SUM(E2:E28)</f>
+        <v>5303.5099999999984</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>74</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1246,8 +1275,9 @@
     <hyperlink ref="D26" r:id="rId24" xr:uid="{078ADCB4-68C8-47D6-921B-BFCF3D41E25D}"/>
     <hyperlink ref="D27" r:id="rId25" xr:uid="{D0FFA605-99F2-48D2-A9AC-D83405F41AFA}"/>
     <hyperlink ref="D25" r:id="rId26" xr:uid="{0958646A-9138-4386-A3D4-B440EC4F598E}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{02C480C3-4EA3-4300-9045-F5E06740F360}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId27"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Home Depot order for wire strippers to expense report
</commit_message>
<xml_diff>
--- a/Ordered Parts/Expense Report.xlsx
+++ b/Ordered Parts/Expense Report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B1486A-8DCD-4F73-A67A-B96462D95160}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B955E9D7-AE10-4550-BCEC-3298BF718705}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="106">
   <si>
     <t>Description</t>
   </si>
@@ -329,6 +329,15 @@
   </si>
   <si>
     <t>Heat Shrink Tubing</t>
+  </si>
+  <si>
+    <t>Home Depot Order</t>
+  </si>
+  <si>
+    <t>Home Depot Order 1.pdf</t>
+  </si>
+  <si>
+    <t>Wire Strippers</t>
   </si>
 </sst>
 </file>
@@ -675,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1314,24 +1323,44 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D32" s="1" t="s">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="5">
+        <v>43191</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="6">
+        <v>30.43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="6">
-        <f>SUM(E2:E31)</f>
-        <v>5341.869999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="D33" t="s">
+      <c r="E33" s="6">
+        <f>SUM(E2:E32)</f>
+        <v>5372.2999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D34" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
         <v>74</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1367,8 +1396,9 @@
     <hyperlink ref="D30" r:id="rId28" xr:uid="{10CD31AD-9521-440C-BFF5-98804EEE03E3}"/>
     <hyperlink ref="D29" r:id="rId29" xr:uid="{F5884C4A-BCCB-45D9-98B2-E0D53C7BF42B}"/>
     <hyperlink ref="D31" r:id="rId30" xr:uid="{BFF74409-40F7-46E8-AF11-01AE4E7DFE63}"/>
+    <hyperlink ref="D32" r:id="rId31" xr:uid="{1892216A-82C2-478E-876D-903829C63D10}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId31"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalized expense report for submission to Georgia Tech
</commit_message>
<xml_diff>
--- a/Ordered Parts/Expense Report.xlsx
+++ b/Ordered Parts/Expense Report.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B955E9D7-AE10-4550-BCEC-3298BF718705}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDD5279-382A-485F-9360-8B5055C25EB0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
   <si>
     <t>Description</t>
   </si>
@@ -121,9 +121,6 @@
     <t xml:space="preserve">Soldering Station, Tip Cleaner, Tip Tinner, Extra Iron Tips </t>
   </si>
   <si>
-    <t>Amazon Order 6*</t>
-  </si>
-  <si>
     <t>Banggood Order 1</t>
   </si>
   <si>
@@ -244,12 +241,6 @@
     <t>Mounting screws, nuts, and standoffs, AC/DC Power Adapter, Programming Cable, and Ball Bearings</t>
   </si>
   <si>
-    <t>*Not sure whether to expense this order</t>
-  </si>
-  <si>
-    <t>Hobby King Order 4.pdf**</t>
-  </si>
-  <si>
     <t>Amazon Order 10</t>
   </si>
   <si>
@@ -259,12 +250,6 @@
     <t>Female PCB Headers, 2mm Bullet Plugs, M3 screws</t>
   </si>
   <si>
-    <t>Amazon Order 9.pdf***</t>
-  </si>
-  <si>
-    <t>**Refunded $23.58 after 2 motors were out of stock</t>
-  </si>
-  <si>
     <t>Arrow Order 5</t>
   </si>
   <si>
@@ -319,9 +304,6 @@
     <t>12V Finalized Power Adapters</t>
   </si>
   <si>
-    <t>***Refunded $8.18 for an incorrect shipment, an additional $326.00 for returned USB cables, and another $999.00 for returned power adapters</t>
-  </si>
-  <si>
     <t>Amazon Order 15</t>
   </si>
   <si>
@@ -338,6 +320,21 @@
   </si>
   <si>
     <t>Wire Strippers</t>
+  </si>
+  <si>
+    <t>*Refunded $23.58 after 2 motors were out of stock</t>
+  </si>
+  <si>
+    <t>**Refunded $8.18 for an incorrect shipment, an additional $326.00 for returned USB cables, and another $999.00 for returned power adapters</t>
+  </si>
+  <si>
+    <t>Hobby King Order 4.pdf*</t>
+  </si>
+  <si>
+    <t>Amazon Order 9.pdf**</t>
+  </si>
+  <si>
+    <t>Amazon Order 6</t>
   </si>
 </sst>
 </file>
@@ -686,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -862,7 +859,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="5">
         <v>43084</v>
@@ -871,7 +868,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="6">
         <v>52.58</v>
@@ -882,7 +879,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5">
         <v>43084</v>
@@ -891,7 +888,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="6">
         <v>45.22</v>
@@ -902,7 +899,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="B11" s="5">
         <v>43084</v>
@@ -922,7 +919,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5">
         <v>43092</v>
@@ -931,18 +928,18 @@
         <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="6">
         <v>23.08</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5">
         <v>43096</v>
@@ -951,18 +948,18 @@
         <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="6">
         <v>74.790000000000006</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="5">
         <v>43097</v>
@@ -971,18 +968,18 @@
         <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="6">
         <v>21.51</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="5">
         <v>43117</v>
@@ -991,18 +988,18 @@
         <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="6">
         <v>24.74</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5">
         <v>43136</v>
@@ -1011,18 +1008,18 @@
         <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="6">
         <v>42.37</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="5">
         <v>43136</v>
@@ -1031,18 +1028,18 @@
         <v>7</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="6">
         <v>17.29</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="5">
         <v>43136</v>
@@ -1051,100 +1048,100 @@
         <v>7</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="6">
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="5">
         <v>43150</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="6">
         <v>288.70999999999998</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="5">
         <v>43150</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="E20" s="6">
         <f>2139.12-23.58</f>
         <v>2115.54</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="5">
         <v>43150</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="6">
         <v>387.12</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="5">
         <v>43150</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E22" s="6">
         <f>1537.58-8.18-326-999</f>
         <v>204.39999999999986</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="5">
         <v>43151</v>
@@ -1153,18 +1150,18 @@
         <v>7</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="6">
         <v>35.729999999999997</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B24" s="5">
         <v>43153</v>
@@ -1173,18 +1170,18 @@
         <v>12</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E24" s="6">
         <v>101.29</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B25" s="5">
         <v>43155</v>
@@ -1193,18 +1190,18 @@
         <v>12</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E25" s="6">
         <v>58.73</v>
       </c>
       <c r="F25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B26" s="5">
         <v>43155</v>
@@ -1213,18 +1210,18 @@
         <v>12</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E26" s="6">
         <v>209.04</v>
       </c>
       <c r="F26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B27" s="5">
         <v>43155</v>
@@ -1233,18 +1230,18 @@
         <v>12</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E27" s="6">
         <v>58.07</v>
       </c>
       <c r="F27" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B28" s="5">
         <v>43158</v>
@@ -1253,38 +1250,38 @@
         <v>12</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E28" s="6">
         <v>27.97</v>
       </c>
       <c r="F28" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B29" s="5">
         <v>43164</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E29" s="6">
         <v>995.37</v>
       </c>
       <c r="F29" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B30" s="5">
         <v>43170</v>
@@ -1293,18 +1290,18 @@
         <v>12</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E30" s="6">
         <v>25.01</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B31" s="5">
         <v>43191</v>
@@ -1313,18 +1310,18 @@
         <v>7</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E31" s="6">
         <v>16.98</v>
       </c>
       <c r="F31" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B32" s="5">
         <v>43191</v>
@@ -1333,35 +1330,32 @@
         <v>12</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E32" s="6">
         <v>30.43</v>
       </c>
       <c r="F32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="6">
         <f>SUM(E2:E32)</f>
         <v>5372.2999999999993</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>74</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>